<commit_message>
8 No Gober Beel Khal Complete
8 No Gober Beel Khal Complete
</commit_message>
<xml_diff>
--- a/AEMostofa/Southwest Project/SMO Gopalgonj/Khal/P1/XL DATA/Hydraulogic_Design_output.xlsx
+++ b/AEMostofa/Southwest Project/SMO Gopalgonj/Khal/P1/XL DATA/Hydraulogic_Design_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Design_All_DC_5\AEMostofa\Southwest Project\SMO Gopalgonj\Khal\P1\XL DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF3572A-7EB5-4045-BFA5-4702ABC6DCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5E67BF-7236-45B6-853B-88888C2C8F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S223"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B29"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4867,7 +4867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>